<commit_message>
updating revenue model for vlookup range change
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestRevenue/Model/Revenue_model_changed_V4.xlsx
+++ b/src/test/resources/TestDriver/TestRevenue/Model/Revenue_model_changed_V4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\TestRevenue\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EF1F9-1617-4E9E-BF73-7D155E80EA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A7A8A-A9A7-417D-BD22-EE35F4AC20CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xxJOB" sheetId="10" r:id="rId1"/>
@@ -4745,7 +4745,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -5259,8 +5259,8 @@
   </sheetPr>
   <dimension ref="A1:DD51"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5392,7 +5392,7 @@
         <v/>
       </c>
       <c r="I3" s="13" t="str">
-        <f>IF($A3="","",VLOOKUP(A3,ProductCatalog_Allocation_Calc!$A$3:$D$7,4,FALSE()))</f>
+        <f>IF($A3="","",VLOOKUP(A3,ProductCatalog_Allocation_Calc!$A$3:$D$8,4,FALSE()))</f>
         <v/>
       </c>
       <c r="J3" s="23" t="str">
@@ -5446,7 +5446,7 @@
         <v/>
       </c>
       <c r="I4" s="13" t="str">
-        <f>IF($A4="","",VLOOKUP(A4,ProductCatalog_Allocation_Calc!$A$3:$D$7,4,FALSE()))</f>
+        <f>IF($A4="","",VLOOKUP(A4,ProductCatalog_Allocation_Calc!$A$3:$D$8,4,FALSE()))</f>
         <v/>
       </c>
       <c r="J4" s="23" t="str">
@@ -5497,7 +5497,7 @@
         <v/>
       </c>
       <c r="I5" s="13" t="str">
-        <f>IF($A5="","",VLOOKUP(A5,ProductCatalog_Allocation_Calc!$A$3:$D$7,4,FALSE()))</f>
+        <f>IF($A5="","",VLOOKUP(A5,ProductCatalog_Allocation_Calc!$A$3:$D$8,4,FALSE()))</f>
         <v/>
       </c>
       <c r="J5" s="23" t="str">
@@ -5548,7 +5548,7 @@
         <v/>
       </c>
       <c r="I6" s="13" t="str">
-        <f>IF($A6="","",VLOOKUP(A6,ProductCatalog_Allocation_Calc!$A$3:$D$7,4,FALSE()))</f>
+        <f>IF($A6="","",VLOOKUP(A6,ProductCatalog_Allocation_Calc!$A$3:$D$8,4,FALSE()))</f>
         <v/>
       </c>
       <c r="J6" s="23" t="str">
@@ -5583,7 +5583,7 @@
         <v/>
       </c>
       <c r="E7" s="22" t="str">
-        <f>IF($A7="","",#REF!)</f>
+        <f>IF($A7="","",VLOOKUP(A7,REV!$E$2:$I$8,3,FALSE()))</f>
         <v/>
       </c>
       <c r="F7" s="13" t="str">
@@ -5599,7 +5599,7 @@
         <v/>
       </c>
       <c r="I7" s="13" t="str">
-        <f>IF($A7="","",VLOOKUP(A7,ProductCatalog_Allocation_Calc!$A$3:$D$7,4,FALSE()))</f>
+        <f>IF($A7="","",VLOOKUP(A7,ProductCatalog_Allocation_Calc!$A$3:$D$8,4,FALSE()))</f>
         <v/>
       </c>
       <c r="J7" s="23" t="str">

</xml_diff>